<commit_message>
Added formatting for custom chart data labels.
</commit_message>
<xml_diff>
--- a/test/perl_output/chart_data_labels.xlsx
+++ b/test/perl_output/chart_data_labels.xlsx
@@ -513,7 +513,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Chart with custom string data labels</a:t>
+              <a:t>Data labels with formatting</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -529,108 +529,16 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t>Amy</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showVal val="1"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t>Bea</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showVal val="1"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t>Eva</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showVal val="1"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t>Fay</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showVal val="1"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t>Liv</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showVal val="1"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t>Una</a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:showVal val="1"/>
-            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
             <c:showVal val="1"/>
           </c:dLbls>
           <c:cat>
@@ -744,7 +652,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Chart with custom data labels from cells</a:t>
+              <a:t>Chart with custom string data labels</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -764,15 +672,16 @@
               <c:idx val="0"/>
               <c:layout/>
               <c:tx>
-                <c:strRef>
-                  <c:f>Sheet1!$C$2</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>Jan</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Amy</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
               </c:tx>
               <c:showVal val="1"/>
             </c:dLbl>
@@ -780,15 +689,16 @@
               <c:idx val="1"/>
               <c:layout/>
               <c:tx>
-                <c:strRef>
-                  <c:f>Sheet1!$C$3</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>Feb</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Bea</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
               </c:tx>
               <c:showVal val="1"/>
             </c:dLbl>
@@ -796,15 +706,16 @@
               <c:idx val="2"/>
               <c:layout/>
               <c:tx>
-                <c:strRef>
-                  <c:f>Sheet1!$C$4</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>Mar</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Eva</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
               </c:tx>
               <c:showVal val="1"/>
             </c:dLbl>
@@ -812,15 +723,16 @@
               <c:idx val="3"/>
               <c:layout/>
               <c:tx>
-                <c:strRef>
-                  <c:f>Sheet1!$C$5</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>Apr</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Fay</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
               </c:tx>
               <c:showVal val="1"/>
             </c:dLbl>
@@ -828,15 +740,16 @@
               <c:idx val="4"/>
               <c:layout/>
               <c:tx>
-                <c:strRef>
-                  <c:f>Sheet1!$C$6</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>May</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Liv</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
               </c:tx>
               <c:showVal val="1"/>
             </c:dLbl>
@@ -844,15 +757,16 @@
               <c:idx val="5"/>
               <c:layout/>
               <c:tx>
-                <c:strRef>
-                  <c:f>Sheet1!$C$7</c:f>
-                  <c:strCache>
-                    <c:ptCount val="1"/>
-                    <c:pt idx="0">
-                      <c:v>Jun</c:v>
-                    </c:pt>
-                  </c:strCache>
-                </c:strRef>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Una</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
               </c:tx>
               <c:showVal val="1"/>
             </c:dLbl>
@@ -969,7 +883,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Mixed custom and default data labels</a:t>
+              <a:t>Chart with custom data labels from cells</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -999,21 +913,22 @@
                   </c:strCache>
                 </c:strRef>
               </c:tx>
-              <c:spPr/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr baseline="0">
-                      <a:solidFill>
-                        <a:srgbClr val="FF0000"/>
-                      </a:solidFill>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>Sheet1!$C$3</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>Feb</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
               <c:showVal val="1"/>
             </c:dLbl>
             <c:dLbl>
@@ -1030,21 +945,6 @@
                   </c:strCache>
                 </c:strRef>
               </c:tx>
-              <c:spPr/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr baseline="0">
-                      <a:solidFill>
-                        <a:srgbClr val="FF0000"/>
-                      </a:solidFill>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
               <c:showVal val="1"/>
             </c:dLbl>
             <c:dLbl>
@@ -1061,21 +961,38 @@
                   </c:strCache>
                 </c:strRef>
               </c:tx>
-              <c:spPr/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr baseline="0">
-                      <a:solidFill>
-                        <a:srgbClr val="FF0000"/>
-                      </a:solidFill>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>Sheet1!$C$6</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>May</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>Sheet1!$C$7</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>Jun</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
               <c:showVal val="1"/>
             </c:dLbl>
             <c:showVal val="1"/>
@@ -1191,7 +1108,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Chart with deleted data labels</a:t>
+              <a:t>Mixed custom and default data labels</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1209,19 +1126,96 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:delete val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>Sheet1!$C$2</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>Jan</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:spPr/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showVal val="1"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:delete val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>Sheet1!$C$4</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>Mar</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:spPr/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showVal val="1"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
-              <c:delete val="1"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:delete val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:strRef>
+                  <c:f>Sheet1!$C$5</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>Apr</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:spPr/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showVal val="1"/>
             </c:dLbl>
             <c:showVal val="1"/>
           </c:dLbls>
@@ -1307,6 +1301,410 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50070001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Chart with deleted data labels</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50080001"/>
+        <c:axId val="50080002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50080001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50080002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50080002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50080001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Chart with custom labels and formatting</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Amy</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="0000FF"/>
+                  </a:solidFill>
+                </a:ln>
+              </c:spPr>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Bea</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Eva</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Fay</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Liv</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Una</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="008000"/>
+                </a:solidFill>
+              </c:spPr>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50090001"/>
+        <c:axId val="50090002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50090001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50090002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50090002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50090001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1528,6 +1926,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>

</xml_diff>